<commit_message>
Added LOINC temporary codes
</commit_message>
<xml_diff>
--- a/test cases/Temporary Codes.xlsx
+++ b/test cases/Temporary Codes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sisc\priority\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64196F24-99B3-4C94-9064-13C7402279CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E78A2C-FE6B-43D5-A38D-6C81A1CDB586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{098EC7A3-6ECE-4867-A1D4-8F62C34D7B21}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pandemic" sheetId="3" r:id="rId1"/>
-    <sheet name="Population Groups" sheetId="1" r:id="rId2"/>
-    <sheet name="Tier" sheetId="2" r:id="rId3"/>
+    <sheet name="LOINC" sheetId="4" r:id="rId1"/>
+    <sheet name="Pandemic" sheetId="3" r:id="rId2"/>
+    <sheet name="Population Groups" sheetId="1" r:id="rId3"/>
+    <sheet name="Tier" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>CODE</t>
   </si>
@@ -270,6 +271,27 @@
   </si>
   <si>
     <t>HL7</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TPG_PAND</t>
+  </si>
+  <si>
+    <t>TPG_POP_GRP</t>
+  </si>
+  <si>
+    <t>TPG_TIER</t>
+  </si>
+  <si>
+    <t>Priority Group - Pandemic</t>
+  </si>
+  <si>
+    <t>Priority Group - Population Group</t>
+  </si>
+  <si>
+    <t>Priority Group - Tier</t>
   </si>
 </sst>
 </file>
@@ -649,10 +671,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9CE2DC-4667-405A-ACF7-D03F7048DF7B}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="str">
+        <f>A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <v>TPG_PAND^Priority Group - Pandemic^99TPG</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="str">
+        <f>A3&amp;"^"&amp;SUBSTITUTE(B3, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <v>TPG_POP_GRP^Priority Group - Population Group^99TPG</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="str">
+        <f>A4&amp;"^"&amp;SUBSTITUTE(B4, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <v>TPG_TIER^Priority Group - Tier^99TPG</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637E8CB4-E7A6-4A85-9119-E0270A77B77F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -714,7 +804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E1AD78-E241-46CF-88E6-89556DAEFF4E}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -1081,7 +1171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D4E6F-84DB-4267-9164-FA20AB1FCF9C}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1113,7 +1203,7 @@
         <v>65</v>
       </c>
       <c r="C2" t="str">
-        <f>A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" ref="C2:C7" si="0">A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>T1^Tier 1^99TPG</v>
       </c>
     </row>
@@ -1125,7 +1215,7 @@
         <v>66</v>
       </c>
       <c r="C3" t="str">
-        <f>A3&amp;"^"&amp;SUBSTITUTE(B3, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" si="0"/>
         <v>T2^Tier 2^99TPG</v>
       </c>
     </row>
@@ -1137,7 +1227,7 @@
         <v>67</v>
       </c>
       <c r="C4" t="str">
-        <f>A4&amp;"^"&amp;SUBSTITUTE(B4, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" si="0"/>
         <v>T3^Tier 3^99TPG</v>
       </c>
     </row>
@@ -1149,7 +1239,7 @@
         <v>68</v>
       </c>
       <c r="C5" t="str">
-        <f>A5&amp;"^"&amp;SUBSTITUTE(B5, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" si="0"/>
         <v>T4^Tier 4^99TPG</v>
       </c>
     </row>
@@ -1161,7 +1251,7 @@
         <v>69</v>
       </c>
       <c r="C6" t="str">
-        <f>A6&amp;"^"&amp;SUBSTITUTE(B6, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" si="0"/>
         <v>T5^Tier 5^99TPG</v>
       </c>
     </row>
@@ -1173,7 +1263,7 @@
         <v>70</v>
       </c>
       <c r="C7" t="str">
-        <f>A7&amp;"^"&amp;SUBSTITUTE(B7, "&amp;", "\T\")&amp;"^99TPG"</f>
+        <f t="shared" si="0"/>
         <v>TN^Not Targeted^99TPG</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated test case to new dates, added Java support for temporary codes
</commit_message>
<xml_diff>
--- a/test cases/Temporary Codes.xlsx
+++ b/test cases/Temporary Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\sisc\priority\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E78A2C-FE6B-43D5-A38D-6C81A1CDB586}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594F4872-EE5F-44CD-9AE4-04B0DC2276EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{098EC7A3-6ECE-4867-A1D4-8F62C34D7B21}"/>
+    <workbookView xWindow="3420" yWindow="3435" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{098EC7A3-6ECE-4867-A1D4-8F62C34D7B21}"/>
   </bookViews>
   <sheets>
     <sheet name="LOINC" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>CODE</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Priority Group - Tier</t>
+  </si>
+  <si>
+    <t>JAVA</t>
   </si>
 </sst>
 </file>
@@ -672,20 +675,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9CE2DC-4667-405A-ACF7-D03F7048DF7B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,8 +698,11 @@
       <c r="C1" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -707,8 +713,12 @@
         <f>A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>TPG_PAND^Priority Group - Pandemic^99TPG</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>A2&amp;"("&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;"),"</f>
+        <v>TPG_PAND("TPG_PAND", "Priority Group - Pandemic"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -719,8 +729,12 @@
         <f>A3&amp;"^"&amp;SUBSTITUTE(B3, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>TPG_POP_GRP^Priority Group - Population Group^99TPG</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D4" si="0">A3&amp;"("&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;"),"</f>
+        <v>TPG_POP_GRP("TPG_POP_GRP", "Priority Group - Population Group"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -730,6 +744,10 @@
       <c r="C4" t="str">
         <f>A4&amp;"^"&amp;SUBSTITUTE(B4, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>TPG_TIER^Priority Group - Tier^99TPG</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>TPG_TIER("TPG_TIER", "Priority Group - Tier"),</v>
       </c>
     </row>
   </sheetData>
@@ -740,19 +758,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637E8CB4-E7A6-4A85-9119-E0270A77B77F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +781,11 @@
       <c r="C1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -774,8 +796,12 @@
         <f>A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>P2020-FLU^Pandemic 2020 - Influenza^99TPG</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(A2, "-", "_")&amp;"("&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;"),"</f>
+        <v>P2020_FLU("P2020-FLU", "Pandemic 2020 - Influenza"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -786,8 +812,12 @@
         <f>A3&amp;"^"&amp;SUBSTITUTE(B3, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>P2020-COVID^Pandemic 2020 - COVID^99TPG</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D4" si="0">SUBSTITUTE(A3, "-", "_")&amp;"("&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;"),"</f>
+        <v>P2020_COVID("P2020-COVID", "Pandemic 2020 - COVID"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -797,6 +827,10 @@
       <c r="C4" t="str">
         <f>A4&amp;"^"&amp;SUBSTITUTE(B4, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>P2020-TX-HURRICANE^Pandemic 2020 - Texas Hurricane Disaster^99TPG</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>P2020_TX_HURRICANE("P2020-TX-HURRICANE", "Pandemic 2020 - Texas Hurricane Disaster"),</v>
       </c>
     </row>
   </sheetData>
@@ -806,19 +840,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E1AD78-E241-46CF-88E6-89556DAEFF4E}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -828,8 +863,11 @@
       <c r="C1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -840,8 +878,12 @@
         <f>A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>PG01^Deployed \T\ mission essential personnel^99TPG</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(A2, "-", "_")&amp;"("&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;"),"</f>
+        <v>PG01("PG01", "Deployed &amp; mission essential personnel"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -852,8 +894,12 @@
         <f t="shared" ref="C3:C29" si="0">A3&amp;"^"&amp;SUBSTITUTE(B3, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>PG02^Essential military support \T\ sustainment personnel^99TPG</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D29" si="1">SUBSTITUTE(A3, "-", "_")&amp;"("&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;"),"</f>
+        <v>PG02("PG02", "Essential military support &amp; sustainment personnel"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -864,8 +910,12 @@
         <f t="shared" si="0"/>
         <v>PG03^Intelligence services^99TPG</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>PG03("PG03", "Intelligence services"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -876,8 +926,12 @@
         <f t="shared" si="0"/>
         <v>PG04^National Guard personne^99TPG</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>PG04("PG04", "National Guard personne"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -888,8 +942,12 @@
         <f t="shared" si="0"/>
         <v>PG05^Other domestic national security personnel^99TPG</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>PG05("PG05", "Other domestic national security personnel"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -900,8 +958,12 @@
         <f t="shared" si="0"/>
         <v>PG06^Other active duty military \T\ essential support^99TPG</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>PG06("PG06", "Other active duty military &amp; essential support"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -912,8 +974,12 @@
         <f t="shared" si="0"/>
         <v>PG07^Public health personnel^99TPG</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>PG07("PG07", "Public health personnel"),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -924,8 +990,12 @@
         <f t="shared" si="0"/>
         <v>PG08^Inpatient health care providers^99TPG</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>PG08("PG08", "Inpatient health care providers"),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
@@ -936,8 +1006,12 @@
         <f t="shared" si="0"/>
         <v>PG09^Outpatient \T\ home health providers^99TPG</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>PG09("PG09", "Outpatient &amp; home health providers"),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -948,8 +1022,12 @@
         <f t="shared" si="0"/>
         <v>PG10^Health care providers in long-term care facilities^99TPG</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>PG10("PG10", "Health care providers in long-term care facilities"),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -960,8 +1038,12 @@
         <f t="shared" si="0"/>
         <v>PG11^Pharmacists \T\ pharmacy technicians^99TPG</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>PG11("PG11", "Pharmacists &amp; pharmacy technicians"),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -972,8 +1054,12 @@
         <f t="shared" si="0"/>
         <v>PG12^Community support \T\ emergency management^99TPG</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>PG12("PG12", "Community support &amp; emergency management"),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
@@ -984,8 +1070,12 @@
         <f t="shared" si="0"/>
         <v>PG13^Mortuary services personnel^99TPG</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>PG13("PG13", "Mortuary services personnel"),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -996,8 +1086,12 @@
         <f t="shared" si="0"/>
         <v>PG14^Other health care personnel^99TPG</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>PG14("PG14", "Other health care personnel"),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -1008,8 +1102,12 @@
         <f t="shared" si="0"/>
         <v>PG15^Emergency services \T\ public safety sector personnel (EMS, law enforcement, \T\ fire services)^99TPG</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>PG15("PG15", "Emergency services &amp; public safety sector personnel (EMS, law enforcement, &amp; fire services)"),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -1020,8 +1118,12 @@
         <f t="shared" si="0"/>
         <v>PG16^Manufacturers of pandemic vaccine \T\ antivirals^99TPG</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>PG16("PG16", "Manufacturers of pandemic vaccine &amp; antivirals"),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -1032,8 +1134,12 @@
         <f t="shared" si="0"/>
         <v>PG17^Communications/information technology (IT), electricity, nuclear, oil \T\ gas, water sector personnel, \T\ financial clearing \T\ settlement personnel^99TPG</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>PG17("PG17", "Communications/information technology (IT), electricity, nuclear, oil &amp; gas, water sector personnel, &amp; financial clearing &amp; settlement personnel"),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -1044,8 +1150,12 @@
         <f t="shared" si="0"/>
         <v>PG18^Critical government personnel - operational \T\ regulatory functions^99TPG</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>PG18("PG18", "Critical government personnel - operational &amp; regulatory functions"),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1056,8 +1166,12 @@
         <f t="shared" si="0"/>
         <v>PG19^Banking \T\ finance, chemical, food \T\ agriculture, pharmaceutical, postal \T\ shipping, \T\ transportation sector personnel (critical infrastructure with greater redundancy)^99TPG</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>PG19("PG19", "Banking &amp; finance, chemical, food &amp; agriculture, pharmaceutical, postal &amp; shipping, &amp; transportation sector personnel (critical infrastructure with greater redundancy)"),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
@@ -1068,8 +1182,12 @@
         <f t="shared" si="0"/>
         <v>PG20^Other critical government personnel^99TPG</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>PG20("PG20", "Other critical government personnel"),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
@@ -1080,8 +1198,12 @@
         <f t="shared" si="0"/>
         <v>PG21^Pregnant women^99TPG</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>PG21("PG21", "Pregnant women"),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1092,8 +1214,12 @@
         <f t="shared" si="0"/>
         <v>PG22^Infants \T\ toddlers 6-35 months old^99TPG</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>PG22("PG22", "Infants &amp; toddlers 6-35 months old"),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
@@ -1104,8 +1230,12 @@
         <f t="shared" si="0"/>
         <v>PG23^Household contacts of infants^99TPG</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>PG23("PG23", "Household contacts of infants"),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>52</v>
       </c>
@@ -1116,8 +1246,12 @@
         <f t="shared" si="0"/>
         <v>PG24^Children 3-18 years old with high risk condition^99TPG</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>PG24("PG24", "Children 3-18 years old with high risk condition"),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1128,8 +1262,12 @@
         <f t="shared" si="0"/>
         <v>PG25^Children 3-18 years old without high risk condition^99TPG</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>PG25("PG25", "Children 3-18 years old without high risk condition"),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>54</v>
       </c>
@@ -1140,8 +1278,12 @@
         <f t="shared" si="0"/>
         <v>PG26^Adults 19-64 years old with high risk condition^99TPG</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>PG26("PG26", "Adults 19-64 years old with high risk condition"),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>55</v>
       </c>
@@ -1152,8 +1294,12 @@
         <f t="shared" si="0"/>
         <v>PG27^Adults &gt;65 years old^99TPG</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>PG27("PG27", "Adults &gt;65 years old"),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>56</v>
       </c>
@@ -1163,6 +1309,10 @@
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>PG28^Healthy adults 19-64 years old^99TPG</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>PG28("PG28", "Healthy adults 19-64 years old"),</v>
       </c>
     </row>
   </sheetData>
@@ -1173,18 +1323,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D4E6F-84DB-4267-9164-FA20AB1FCF9C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,8 +1346,11 @@
       <c r="C1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1206,8 +1361,12 @@
         <f t="shared" ref="C2:C7" si="0">A2&amp;"^"&amp;SUBSTITUTE(B2, "&amp;", "\T\")&amp;"^99TPG"</f>
         <v>T1^Tier 1^99TPG</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>SUBSTITUTE(A2, "-", "_")&amp;"("&amp;CHAR(34)&amp;A2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;"),"</f>
+        <v>T1("T1", "Tier 1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1218,8 +1377,12 @@
         <f t="shared" si="0"/>
         <v>T2^Tier 2^99TPG</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D7" si="1">SUBSTITUTE(A3, "-", "_")&amp;"("&amp;CHAR(34)&amp;A3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;"),"</f>
+        <v>T2("T2", "Tier 2"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1230,8 +1393,12 @@
         <f t="shared" si="0"/>
         <v>T3^Tier 3^99TPG</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>T3("T3", "Tier 3"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1242,8 +1409,12 @@
         <f t="shared" si="0"/>
         <v>T4^Tier 4^99TPG</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>T4("T4", "Tier 4"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1254,8 +1425,12 @@
         <f t="shared" si="0"/>
         <v>T5^Tier 5^99TPG</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>T5("T5", "Tier 5"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1265,6 +1440,10 @@
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>TN^Not Targeted^99TPG</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>TN("TN", "Not Targeted"),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>